<commit_message>
add java package info to Excel file
as Namespace
</commit_message>
<xml_diff>
--- a/EntityDefinition.xlsx
+++ b/EntityDefinition.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="62">
   <si>
     <t>EntityName</t>
   </si>
@@ -27,6 +27,12 @@
     <t>Common meta columns</t>
   </si>
   <si>
+    <t>Namespace</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
     <t>Columns</t>
   </si>
   <si>
@@ -96,6 +102,9 @@
     <t>Employee Description is here.</t>
   </si>
   <si>
+    <t>com.shionit.model</t>
+  </si>
+  <si>
     <t>EnumType</t>
   </si>
   <si>
@@ -145,6 +154,9 @@
   </si>
   <si>
     <t>EnumDescription</t>
+  </si>
+  <si>
+    <t>com.shionit.model.enums</t>
   </si>
   <si>
     <t>Entries</t>
@@ -245,11 +257,17 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -259,9 +277,6 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -517,72 +532,64 @@
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3" t="s">
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="C5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="D5" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="s">
+      <c r="E5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="F5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="2">
-        <v>128.0</v>
-      </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="D6" s="2">
+        <v>128.0</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="2">
-        <v>128.0</v>
-      </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
@@ -592,11 +599,13 @@
         <v>20</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="D8" s="2">
+        <v>128.0</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
@@ -606,101 +615,115 @@
         <v>22</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
+      <c r="C10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="6"/>
     </row>
     <row r="11">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
     </row>
     <row r="12">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
     </row>
     <row r="13">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
     </row>
     <row r="14">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
     </row>
     <row r="15">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
     </row>
     <row r="16">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
     </row>
     <row r="17">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
     </row>
     <row r="18">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
     </row>
     <row r="19">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
     </row>
     <row r="20">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -726,67 +749,56 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="B3" s="4" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="6" t="s">
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="E5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G5" s="4"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
@@ -796,29 +808,33 @@
         <v>32</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="2">
-        <v>128.0</v>
-      </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+        <v>33</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="G6" s="6"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="D7" s="2">
+        <v>128.0</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
@@ -830,126 +846,141 @@
       <c r="C8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="2" t="s">
-        <v>39</v>
-      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="2" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+      <c r="A10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
     </row>
     <row r="11">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
     </row>
     <row r="12">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
     </row>
     <row r="13">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
     </row>
     <row r="14">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
     </row>
     <row r="15">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
     </row>
     <row r="16">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
     </row>
     <row r="17">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
     </row>
     <row r="18">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
     </row>
     <row r="19">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
     </row>
     <row r="20">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -972,100 +1003,108 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>37</v>
+      <c r="A2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="6" t="s">
-        <v>44</v>
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>45</v>
+      <c r="A4" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="A5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="4">
         <v>1.0</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="2">
+    <row r="7">
+      <c r="A7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="4">
         <v>2.0</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" s="2">
+    <row r="8">
+      <c r="A8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="4">
         <v>3.0</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="2">
+    <row r="9">
+      <c r="A9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="4">
         <v>4.0</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" s="2">
+    <row r="10">
+      <c r="A10" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="4">
         <v>5.0</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" s="2">
+    <row r="11">
+      <c r="A11" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="4">
         <v>6.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add Java Entity Annotations
- add Lombok and JPA Annotations to java Entities
- add TestCase
</commit_message>
<xml_diff>
--- a/EntityDefinition.xlsx
+++ b/EntityDefinition.xlsx
@@ -5,7 +5,8 @@
   <sheets>
     <sheet state="visible" name="META" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="EMPLOYEE" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="EmployeeRank" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="SOMETHING" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="EmployeeRank" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -13,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="72">
   <si>
     <t>EntityName</t>
   </si>
@@ -148,6 +149,37 @@
   </si>
   <si>
     <t>True if the employee exited.</t>
+  </si>
+  <si>
+    <t>SOMETHING</t>
+  </si>
+  <si>
+    <t>Something Entity test data.
+no Length, no NotNull, multi PK, no Enum.</t>
+  </si>
+  <si>
+    <t>INT_COL</t>
+  </si>
+  <si>
+    <t>int column.</t>
+  </si>
+  <si>
+    <t>DATE_COL</t>
+  </si>
+  <si>
+    <t>date column.</t>
+  </si>
+  <si>
+    <t>DATETIME_COL</t>
+  </si>
+  <si>
+    <t>datetime column.</t>
+  </si>
+  <si>
+    <t>BOOL_COL</t>
+  </si>
+  <si>
+    <t>boolean column.</t>
   </si>
   <si>
     <t>EnumName</t>
@@ -297,6 +329,10 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -810,7 +846,7 @@
       <c r="C6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="6"/>
+      <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
         <v>26</v>
       </c>
@@ -999,12 +1035,259 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="19.14"/>
     <col customWidth="1" min="2" max="2" width="29.29"/>
+    <col customWidth="1" min="3" max="3" width="17.0"/>
+    <col customWidth="1" min="4" max="4" width="10.43"/>
+    <col customWidth="1" min="5" max="5" width="9.86"/>
+    <col customWidth="1" min="6" max="6" width="9.57"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="19.14"/>
+    <col customWidth="1" min="2" max="2" width="29.29"/>
     <col customWidth="1" min="3" max="3" width="11.86"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>42</v>
@@ -1012,7 +1295,7 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>40</v>
@@ -1023,12 +1306,12 @@
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="7" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5">
@@ -1039,15 +1322,15 @@
         <v>8</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="C6" s="4">
         <v>1.0</v>
@@ -1055,10 +1338,10 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C7" s="4">
         <v>2.0</v>
@@ -1066,10 +1349,10 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="C8" s="4">
         <v>3.0</v>
@@ -1077,10 +1360,10 @@
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="C9" s="4">
         <v>4.0</v>
@@ -1088,10 +1371,10 @@
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C10" s="4">
         <v>5.0</v>
@@ -1099,10 +1382,10 @@
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="C11" s="4">
         <v>6.0</v>

</xml_diff>

<commit_message>
feat format Enum Column correctly
</commit_message>
<xml_diff>
--- a/EntityDefinition.xlsx
+++ b/EntityDefinition.xlsx
@@ -227,10 +227,10 @@
     <t>principal.</t>
   </si>
   <si>
-    <t>PERTNER</t>
-  </si>
-  <si>
-    <t>pertner.</t>
+    <t>PARTNER</t>
+  </si>
+  <si>
+    <t>partner.</t>
   </si>
 </sst>
 </file>
@@ -289,7 +289,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -299,17 +299,11 @@
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -565,35 +559,35 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -610,8 +604,8 @@
       <c r="D6" s="2">
         <v>128.0</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
@@ -624,8 +618,8 @@
         <v>18</v>
       </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
@@ -640,8 +634,8 @@
       <c r="D8" s="2">
         <v>128.0</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
@@ -654,8 +648,8 @@
         <v>18</v>
       </c>
       <c r="D9" s="2"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
@@ -667,99 +661,99 @@
       <c r="C10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="6"/>
+      <c r="D10" s="4"/>
       <c r="E10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="6"/>
+      <c r="F10" s="4"/>
     </row>
     <row r="11">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
     </row>
     <row r="12">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
     </row>
     <row r="13">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
     </row>
     <row r="14">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
     </row>
     <row r="15">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
     </row>
     <row r="16">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
     </row>
     <row r="17">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
     </row>
     <row r="18">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
     </row>
     <row r="19">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
     </row>
     <row r="20">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
     </row>
     <row r="21">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -801,38 +795,38 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="3" t="s">
         <v>30</v>
       </c>
     </row>
@@ -846,14 +840,14 @@
       <c r="C6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4" t="s">
+      <c r="D6" s="5"/>
+      <c r="E6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="2">
         <v>1.0</v>
       </c>
-      <c r="G6" s="6"/>
+      <c r="G6" s="4"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
@@ -868,9 +862,9 @@
       <c r="D7" s="2">
         <v>128.0</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
@@ -882,10 +876,10 @@
       <c r="C8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
@@ -897,9 +891,9 @@
       <c r="C9" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
       <c r="G9" s="2" t="s">
         <v>42</v>
       </c>
@@ -914,109 +908,109 @@
       <c r="C10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
     </row>
     <row r="11">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
     </row>
     <row r="12">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
     </row>
     <row r="13">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
     </row>
     <row r="14">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
     </row>
     <row r="15">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
     </row>
     <row r="16">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
     </row>
     <row r="17">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
     </row>
     <row r="18">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
     </row>
     <row r="19">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
     </row>
     <row r="20">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
     </row>
     <row r="21">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1045,7 +1039,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1053,7 +1047,7 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1066,204 +1060,204 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4">
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5">
         <v>1.0</v>
       </c>
-      <c r="G6" s="6"/>
+      <c r="G6" s="4"/>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="4">
+      <c r="D7" s="5"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="5">
         <v>2.0</v>
       </c>
-      <c r="G7" s="6"/>
+      <c r="G7" s="4"/>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="5"/>
     </row>
     <row r="10">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
     </row>
     <row r="11">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
     </row>
     <row r="12">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
     </row>
     <row r="13">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
     </row>
     <row r="14">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
     </row>
     <row r="15">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
     </row>
     <row r="16">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
     </row>
     <row r="17">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
     </row>
     <row r="18">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
     </row>
     <row r="19">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
     </row>
     <row r="20">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
     </row>
     <row r="21">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1286,108 +1280,108 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="3" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="3" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="2">
         <v>1.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="2">
         <v>3.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="2">
         <v>4.0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="2">
         <v>5.0</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="2">
         <v>6.0</v>
       </c>
     </row>

</xml_diff>